<commit_message>
Initial commit v1p3, R2019b
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Power/Electric3Motor/sm_car_data_Power_Electric3Motor.xlsx
+++ b/Libraries/Vehicle/Power/Electric3Motor/sm_car_data_Power_Electric3Motor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\simscape\demos\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Power\Electric3Motor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32014A41-D98F-4B8C-90A2-8C7BBDAE8365}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D13D169-8D4E-45F5-9833-2E6473C9C8CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3EB3AC41-B7D3-4E4D-A710-77CB91E8EAF9}"/>
   </bookViews>
@@ -663,11 +663,11 @@
   <dimension ref="A1:AA138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10:U10"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Initial commit v1p3, R2020a
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Power/Electric3Motor/sm_car_data_Power_Electric3Motor.xlsx
+++ b/Libraries/Vehicle/Power/Electric3Motor/sm_car_data_Power_Electric3Motor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\simscape\demos\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Power\Electric3Motor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D13D169-8D4E-45F5-9833-2E6473C9C8CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32014A41-D98F-4B8C-90A2-8C7BBDAE8365}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3EB3AC41-B7D3-4E4D-A710-77CB91E8EAF9}"/>
   </bookViews>
@@ -663,11 +663,11 @@
   <dimension ref="A1:AA138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10:U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>